<commit_message>
fix merge matrix bug
</commit_message>
<xml_diff>
--- a/src/main/resources/SZ300378.xlsx
+++ b/src/main/resources/SZ300378.xlsx
@@ -64,360 +64,370 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>20181012</t>
+          <t>20181011</t>
         </is>
       </c>
       <c r="B1" t="n">
-        <v>845.0</v>
+        <v>958.0</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>20181122</t>
+          <t>20181012</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1168.0</v>
+        <v>845.0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>20181225</t>
+          <t>20181122</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>936.0</v>
+        <v>1168.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>20190116</t>
+          <t>20181225</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1108.0</v>
+        <v>936.0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>20190130</t>
+          <t>20190116</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>960.0</v>
+        <v>1108.0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>20190312</t>
+          <t>20190130</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1604.0</v>
+        <v>960.0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>20190327</t>
+          <t>20190312</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1276.0</v>
+        <v>1604.0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>20190410</t>
+          <t>20190327</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>2584.0</v>
+        <v>1276.0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>20190508</t>
+          <t>20190410</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>1431.0</v>
+        <v>2584.0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>20190515</t>
+          <t>20190508</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>1615.0</v>
+        <v>1431.0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>20190708</t>
+          <t>20190515</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>1301.0</v>
+        <v>1615.0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>20190802</t>
+          <t>20190708</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>1645.0</v>
+        <v>1301.0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>20190815</t>
+          <t>20190802</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>1310.0</v>
+        <v>1645.0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>20190910</t>
+          <t>20190815</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>1907.0</v>
+        <v>1310.0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>20191021</t>
+          <t>20190910</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>1497.0</v>
+        <v>1907.0</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>20191028</t>
+          <t>20191021</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>1664.0</v>
+        <v>1497.0</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>20191113</t>
+          <t>20191028</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>1382.0</v>
+        <v>1664.0</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>20191120</t>
+          <t>20191113</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>1495.0</v>
+        <v>1382.0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>20191129</t>
+          <t>20191120</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>1322.0</v>
+        <v>1495.0</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>20191218</t>
+          <t>20191129</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>1547.0</v>
+        <v>1322.0</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>20191230</t>
+          <t>20191218</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>1413.0</v>
+        <v>1547.0</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>20200117</t>
+          <t>20191230</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>1675.0</v>
+        <v>1413.0</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>20200204</t>
+          <t>20200117</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>1220.0</v>
+        <v>1675.0</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>20200305</t>
+          <t>20200204</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>1959.0</v>
+        <v>1220.0</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>20200317</t>
+          <t>20200305</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>1551.0</v>
+        <v>1959.0</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>20200326</t>
+          <t>20200317</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>1779.0</v>
+        <v>1551.0</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>20200525</t>
+          <t>20200326</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>1207.0</v>
+        <v>1779.0</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>20200608</t>
+          <t>20200525</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>1308.0</v>
+        <v>1207.0</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>20200612</t>
+          <t>20200608</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>1230.0</v>
+        <v>1308.0</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>20200810</t>
+          <t>20200612</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>4064.0</v>
+        <v>1230.0</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>20200928</t>
+          <t>20200810</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>2640.0</v>
+        <v>4064.0</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>20201012</t>
+          <t>20200928</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>2937.0</v>
+        <v>2640.0</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>20201029</t>
+          <t>20201012</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>2274.0</v>
+        <v>2937.0</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>20201124</t>
+          <t>20201029</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>3245.0</v>
+        <v>2274.0</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>20201202</t>
+          <t>20201124</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>2724.0</v>
+        <v>3245.0</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
+          <t>20201202</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>2724.0</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
           <t>20201215</t>
         </is>
       </c>
-      <c r="B36" t="n">
+      <c r="B37" t="n">
         <v>3186.0</v>
       </c>
     </row>

</xml_diff>